<commit_message>
Atualiza dados da documentação conforme telas wireframe See #50
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F894AF-299E-49E8-90A5-335B19CC5466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17925" windowHeight="9000"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano de ação" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -54,9 +55,6 @@
   </si>
   <si>
     <t>Término - Realizado</t>
-  </si>
-  <si>
-    <t>Homologação da Consulta</t>
   </si>
   <si>
     <t>Enviar especificação para análise da Prodemge</t>
@@ -75,9 +73,6 @@
 1ª versão</t>
   </si>
   <si>
-    <t>Apresentar para a chefia pontos de destaque da especificicação</t>
-  </si>
-  <si>
     <t>Documentação
 Especificação</t>
   </si>
@@ -104,9 +99,6 @@
     <t>DTA/Silviana e Késia</t>
   </si>
   <si>
-    <t>Apresentar para a chefia pontos de destaque da documentação</t>
-  </si>
-  <si>
     <t>Aprovar especificação layout e dados (Monte sua pesquisa)</t>
   </si>
   <si>
@@ -116,35 +108,65 @@
     <t>Especificação de layout e Dados</t>
   </si>
   <si>
-    <t>Homologar Especificação pdsoo</t>
-  </si>
-  <si>
-    <t>Homologação</t>
-  </si>
-  <si>
-    <t>Homologar especificação</t>
-  </si>
-  <si>
     <t>DTA/ Silviana</t>
   </si>
   <si>
-    <t>Homologar protótipo com o cliente</t>
-  </si>
-  <si>
     <t>Homologar protótipo</t>
   </si>
   <si>
-    <t>Homologar consulta - Ambiente de homologação</t>
-  </si>
-  <si>
-    <t>Homologar consulta - Ambiente de produção</t>
+    <t>Apresentação Wireframe</t>
+  </si>
+  <si>
+    <t>Apresentação da Proposta de Protótipo</t>
+  </si>
+  <si>
+    <t>Prodemge</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Homologar telas wireframe</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Revisar especificação de layout</t>
+  </si>
+  <si>
+    <t>Revisar especificação de Dados</t>
+  </si>
+  <si>
+    <t>Apresentar para a chefia pontos de destaque da documentação Layout / Dados</t>
+  </si>
+  <si>
+    <t>Disponibilizar Protótipo - Casos de Uso</t>
+  </si>
+  <si>
+    <t>Protótipo - Casos de Uso</t>
+  </si>
+  <si>
+    <t>Homologação - Entrega 1</t>
+  </si>
+  <si>
+    <t>Homologação - Entrega 3</t>
+  </si>
+  <si>
+    <t>Homologar Consulta</t>
+  </si>
+  <si>
+    <t>Disponibilizar consulta em homologação</t>
+  </si>
+  <si>
+    <t>Homologar consulta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +200,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +219,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -217,11 +253,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -266,13 +303,36 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -549,22 +609,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="23" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="10" max="10" width="30.42578125" customWidth="1"/>
@@ -586,10 +646,10 @@
       <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="14" t="s">
@@ -604,362 +664,443 @@
     </row>
     <row r="2" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="8"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="I2" s="8">
         <v>44588</v>
       </c>
       <c r="J2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="B3" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="18">
+        <v>44596</v>
+      </c>
+      <c r="G3" s="18">
+        <v>44596</v>
+      </c>
+      <c r="H3" s="8">
+        <v>44596</v>
+      </c>
+      <c r="I3" s="8">
+        <v>44596</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="18">
+        <v>44596</v>
+      </c>
+      <c r="G4" s="18">
+        <v>44600</v>
+      </c>
+      <c r="H4" s="8">
+        <v>44596</v>
+      </c>
+      <c r="I4" s="8">
+        <v>44600</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="18">
+        <v>44593</v>
+      </c>
+      <c r="G5" s="18">
+        <v>44603</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7" t="s">
+      <c r="C6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="8">
-        <v>44593</v>
-      </c>
-      <c r="G3" s="8">
-        <v>44600</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="8">
-        <v>44601</v>
-      </c>
-      <c r="G4" s="8">
-        <v>44608</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="F6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="18">
+        <v>44579</v>
+      </c>
+      <c r="H6" s="8">
+        <v>44571</v>
+      </c>
+      <c r="I6" s="8">
+        <v>44588</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8">
-        <v>44579</v>
-      </c>
-      <c r="H5" s="8">
-        <v>44571</v>
-      </c>
-      <c r="I5" s="8">
-        <v>44588</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="8">
-        <v>44595</v>
-      </c>
-      <c r="G6" s="8">
-        <v>44603</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>19</v>
-      </c>
       <c r="C7" s="11" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="8">
+        <v>12</v>
+      </c>
+      <c r="F7" s="18">
         <v>44601</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="18">
         <v>44608</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="8">
-        <v>44609</v>
-      </c>
-      <c r="G8" s="8">
-        <v>44613</v>
+        <v>22</v>
+      </c>
+      <c r="F8" s="18">
+        <v>44595</v>
+      </c>
+      <c r="G8" s="18">
+        <v>44603</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="8">
-        <v>44588</v>
-      </c>
-      <c r="G9" s="16">
-        <v>44594</v>
+        <v>24</v>
+      </c>
+      <c r="F9" s="18">
+        <v>44609</v>
+      </c>
+      <c r="G9" s="18">
+        <v>44613</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="8">
-        <v>44600</v>
-      </c>
-      <c r="G10" s="8">
-        <v>44603</v>
+        <v>30</v>
+      </c>
+      <c r="F10" s="18">
+        <v>44599</v>
+      </c>
+      <c r="G10" s="18">
+        <v>44610</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="8">
-        <v>44637</v>
-      </c>
-      <c r="G11" s="8">
-        <v>44644</v>
+        <v>18</v>
+      </c>
+      <c r="F11" s="18">
+        <v>44610</v>
+      </c>
+      <c r="G11" s="18">
+        <v>44614</v>
       </c>
       <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
+      <c r="I11" s="8"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="8">
-        <v>44650</v>
-      </c>
-      <c r="G12" s="8">
-        <v>44655</v>
-      </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="F12" s="18">
+        <v>44665</v>
+      </c>
+      <c r="G12" s="18">
+        <v>44670</v>
+      </c>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="18">
+        <v>44670</v>
+      </c>
+      <c r="G13" s="20">
+        <v>44673</v>
+      </c>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
       <c r="B16" s="1"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="11"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="5"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="5"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{F3670588-9093-4D73-B964-2C29AC7BAFE5}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Altualiza plano de ação
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F894AF-299E-49E8-90A5-335B19CC5466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5EF1CC-D242-4858-95E5-396DF9D3416A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano de ação" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -90,9 +90,6 @@
 linha 7 cronograma </t>
   </si>
   <si>
-    <t>Revisar especificação e elaborar o filtro 'Monte sua pesquisa'</t>
-  </si>
-  <si>
     <t>Revisar especificação e elaborar dados  'Monte sua pesquisa'</t>
   </si>
   <si>
@@ -160,6 +157,12 @@
   </si>
   <si>
     <t>Homologar consulta</t>
+  </si>
+  <si>
+    <t>Revisar especificação e elaborar o filtro layout'</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
@@ -612,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +684,7 @@
       <c r="F2" s="18"/>
       <c r="G2" s="19"/>
       <c r="H2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="8">
         <v>44588</v>
@@ -695,16 +698,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" s="18">
         <v>44596</v>
@@ -725,16 +728,16 @@
         <v>15</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" s="18">
         <v>44596</v>
@@ -746,23 +749,25 @@
         <v>44596</v>
       </c>
       <c r="I4" s="8">
-        <v>44600</v>
+        <v>44599</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
@@ -772,9 +777,15 @@
       <c r="G5" s="18">
         <v>44603</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="7"/>
+      <c r="H5" s="8">
+        <v>44599</v>
+      </c>
+      <c r="I5" s="8">
+        <v>44599</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -793,7 +804,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6" s="18">
         <v>44579</v>
@@ -816,7 +827,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
@@ -837,14 +848,14 @@
         <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="18">
         <v>44595</v>
@@ -861,14 +872,14 @@
         <v>15</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="18">
         <v>44609</v>
@@ -882,17 +893,17 @@
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="18">
         <v>44599</v>
@@ -906,13 +917,13 @@
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
@@ -930,17 +941,17 @@
     </row>
     <row r="12" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="18">
         <v>44665</v>
@@ -954,13 +965,13 @@
     </row>
     <row r="13" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>41</v>
-      </c>
       <c r="C13" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
@@ -1099,8 +1110,9 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{F3670588-9093-4D73-B964-2C29AC7BAFE5}"/>
+    <hyperlink ref="J5" r:id="rId2" xr:uid="{1E85D808-692D-42AB-BE43-A82A9C0A4D7D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualiza plano de ação - Consulta Vale
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5EF1CC-D242-4858-95E5-396DF9D3416A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A96B980-5F03-41F8-89BE-C260DBCC707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Homologar telas wireframe</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
     <t>Revisar especificação de layout</t>
   </si>
   <si>
@@ -162,7 +159,49 @@
     <t>Revisar especificação e elaborar o filtro layout'</t>
   </si>
   <si>
-    <t>v2</t>
+    <t>Link
+Foram realizadas 3 versões durante a homolgação das telas</t>
+  </si>
+  <si>
+    <t>Especificação tooltip</t>
+  </si>
+  <si>
+    <t>Elaborar documento com os tooltips da consulta</t>
+  </si>
+  <si>
+    <t>DTA/ Késia</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>v2
+Devido a mudanças na extração dos dados é necessário fazer uma nova revisão dos dados</t>
+  </si>
+  <si>
+    <t>atrasada</t>
+  </si>
+  <si>
+    <t>1ª versão apresentada no dia 14/02, é preciso fazer algumas alterações</t>
+  </si>
+  <si>
+    <t>Documentação
+Consulta por Projeto</t>
+  </si>
+  <si>
+    <t>Elaborar documentação da Consulta por Projeto</t>
+  </si>
+  <si>
+    <t>Alinhar com o Comitê os dados da consulta</t>
+  </si>
+  <si>
+    <t>Ficou acordado que a equipe do Comitê irá disponibilizar uma prévia dos dados</t>
+  </si>
+  <si>
+    <t>Elaborar o datapackage da consulta</t>
+  </si>
+  <si>
+    <t>Disponibilizar conjunto no dados.mg</t>
   </si>
 </sst>
 </file>
@@ -261,7 +300,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -329,7 +368,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -337,7 +382,50 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -613,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +718,7 @@
     <col min="7" max="7" width="14.42578125" style="23" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -661,7 +749,7 @@
       <c r="I1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -689,7 +777,7 @@
       <c r="I2" s="8">
         <v>44588</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -721,9 +809,9 @@
       <c r="I3" s="8">
         <v>44596</v>
       </c>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -734,7 +822,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>25</v>
@@ -748,25 +836,23 @@
       <c r="H4" s="8">
         <v>44596</v>
       </c>
-      <c r="I4" s="8">
-        <v>44599</v>
-      </c>
+      <c r="I4" s="8"/>
       <c r="J4" s="24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>12</v>
@@ -784,7 +870,7 @@
         <v>44599</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -815,7 +901,7 @@
       <c r="I6" s="8">
         <v>44588</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="11" t="s">
         <v>14</v>
       </c>
     </row>
@@ -827,9 +913,11 @@
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
@@ -839,21 +927,27 @@
       <c r="G7" s="18">
         <v>44608</v>
       </c>
-      <c r="H7" s="8"/>
+      <c r="H7" s="8">
+        <v>44606</v>
+      </c>
       <c r="I7" s="8"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="11" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="s">
+        <v>49</v>
+      </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
@@ -863,9 +957,11 @@
       <c r="G8" s="18">
         <v>44603</v>
       </c>
-      <c r="H8" s="8"/>
+      <c r="H8" s="8">
+        <v>44603</v>
+      </c>
       <c r="I8" s="8"/>
-      <c r="J8" s="7"/>
+      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
@@ -877,7 +973,9 @@
       <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>23</v>
       </c>
@@ -887,165 +985,223 @@
       <c r="G9" s="18">
         <v>44613</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="8">
+        <v>44606</v>
+      </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="11"/>
+    </row>
+    <row r="10" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="7"/>
+        <v>45</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="E10" s="7" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="F10" s="18">
-        <v>44599</v>
+        <v>44608</v>
       </c>
       <c r="G10" s="18">
-        <v>44610</v>
-      </c>
-      <c r="H10" s="8"/>
+        <v>44613</v>
+      </c>
+      <c r="H10" s="8">
+        <v>44608</v>
+      </c>
       <c r="I10" s="8"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F11" s="18">
+        <v>44599</v>
+      </c>
+      <c r="G11" s="18">
         <v>44610</v>
-      </c>
-      <c r="G11" s="18">
-        <v>44614</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="7"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F12" s="18">
-        <v>44665</v>
+        <v>44610</v>
       </c>
       <c r="G12" s="18">
-        <v>44670</v>
+        <v>44614</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F13" s="18">
+        <v>44665</v>
+      </c>
+      <c r="G13" s="18">
         <v>44670</v>
-      </c>
-      <c r="G13" s="20">
-        <v>44673</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="11"/>
+      <c r="J13" s="11"/>
+    </row>
+    <row r="14" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="E14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="18">
+        <v>44670</v>
+      </c>
+      <c r="G14" s="20">
+        <v>44673</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="J14" s="11"/>
+    </row>
+    <row r="15" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="H15" s="8">
+        <v>44606</v>
+      </c>
+      <c r="I15" s="8">
+        <v>44607</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="18">
+        <v>44613</v>
+      </c>
+      <c r="G16" s="18">
+        <v>44617</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
+      <c r="E17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="18">
+        <v>44627</v>
+      </c>
+      <c r="G17" s="18">
+        <v>44631</v>
+      </c>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1057,7 +1213,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1069,11 +1225,11 @@
       <c r="G20" s="22"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="1"/>
       <c r="C21" s="12"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
@@ -1081,23 +1237,23 @@
       <c r="G21" s="22"/>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="1"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
@@ -1105,12 +1261,35 @@
       <c r="G23" s="22"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="J23" s="12"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="12"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"em andamento"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"concluída"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"atrasada"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{F3670588-9093-4D73-B964-2C29AC7BAFE5}"/>
-    <hyperlink ref="J5" r:id="rId2" xr:uid="{1E85D808-692D-42AB-BE43-A82A9C0A4D7D}"/>
+    <hyperlink ref="J4" r:id="rId1" display="Link" xr:uid="{F3670588-9093-4D73-B964-2C29AC7BAFE5}"/>
+    <hyperlink ref="J5" r:id="rId2" display="v2" xr:uid="{1E85D808-692D-42AB-BE43-A82A9C0A4D7D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Atualiza dados da especificação dados e plano de ação
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A96B980-5F03-41F8-89BE-C260DBCC707E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0B6F5F-AED9-42BE-8F4A-3906D5D459E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -179,9 +179,6 @@
 Devido a mudanças na extração dos dados é necessário fazer uma nova revisão dos dados</t>
   </si>
   <si>
-    <t>atrasada</t>
-  </si>
-  <si>
     <t>1ª versão apresentada no dia 14/02, é preciso fazer algumas alterações</t>
   </si>
   <si>
@@ -202,6 +199,15 @@
   </si>
   <si>
     <t>Disponibilizar conjunto no dados.mg</t>
+  </si>
+  <si>
+    <t>Atrasada</t>
+  </si>
+  <si>
+    <t>planilha com os dados do Projeto</t>
+  </si>
+  <si>
+    <t>Matheus/Cômite</t>
   </si>
 </sst>
 </file>
@@ -386,14 +392,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -421,7 +427,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -701,10 +707,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,7 +828,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>25</v>
@@ -836,7 +842,9 @@
       <c r="H4" s="8">
         <v>44596</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="8">
+        <v>44610</v>
+      </c>
       <c r="J4" s="24" t="s">
         <v>43</v>
       </c>
@@ -852,7 +860,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>12</v>
@@ -916,7 +924,7 @@
         <v>34</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>12</v>
@@ -930,9 +938,11 @@
       <c r="H7" s="8">
         <v>44606</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <v>44610</v>
+      </c>
       <c r="J7" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -946,7 +956,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>21</v>
@@ -960,7 +970,9 @@
       <c r="H8" s="8">
         <v>44603</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <v>44610</v>
+      </c>
       <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -974,7 +986,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>23</v>
@@ -988,7 +1000,9 @@
       <c r="H9" s="8">
         <v>44606</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8">
+        <v>44610</v>
+      </c>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1029,7 +1043,9 @@
       <c r="C11" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="E11" s="7" t="s">
         <v>29</v>
       </c>
@@ -1117,13 +1133,13 @@
     </row>
     <row r="15" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="11" t="s">
         <v>52</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>53</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>13</v>
@@ -1140,80 +1156,92 @@
         <v>44607</v>
       </c>
       <c r="J15" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="8">
+        <v>44607</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="11"/>
+    </row>
+    <row r="17" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="18">
-        <v>44613</v>
-      </c>
-      <c r="G16" s="18">
-        <v>44617</v>
-      </c>
-      <c r="H16" s="8"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="7"/>
       <c r="E17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="18">
+        <v>44613</v>
+      </c>
+      <c r="G17" s="18">
+        <v>44617</v>
+      </c>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="18">
         <v>44627</v>
       </c>
-      <c r="G17" s="18">
+      <c r="G18" s="18">
         <v>44631</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="12"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1241,7 +1269,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="12"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
@@ -1253,8 +1281,8 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="5"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="22"/>
@@ -1265,7 +1293,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -1275,16 +1303,39 @@
       <c r="I24" s="5"/>
       <c r="J24" s="12"/>
     </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="12"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="D1:D15 D17:D1048576">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"atrasada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"concluída"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
       <formula>"em andamento"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"atrasada"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"concluída"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"atrasada"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"em andamento"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Atualiza plano de ação - recursos vale
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD18EE45-A7E9-4005-A24E-E13791CD98CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC87D8-A55A-4F13-8947-0CE3B7B7BA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano de ação" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -223,10 +223,46 @@
     <t>Homologar protótipo monte sua pesquisa</t>
   </si>
   <si>
-    <t>Pendente a valiadaão com o cojunto de dados do Mateus</t>
-  </si>
-  <si>
-    <t>1ª versão dia 03/03/22</t>
+    <t>1ª versão dia 03/03/22
+2ª versão dia 18/03/22</t>
+  </si>
+  <si>
+    <t>1ª versão entregue dia 08/03/22
+2ª versão entregue dia 21/03/22</t>
+  </si>
+  <si>
+    <t>Layout alinhado com a equipe do Comitê. Após treinamento da DTA a equipe passará atualizar os dados diretamente no GitHub</t>
+  </si>
+  <si>
+    <t>O fluxo de atualização foi finalizado com o apoio do Gabriel.
+Pendente criação do repositório no ambiente de produção</t>
+  </si>
+  <si>
+    <t>04/04/2022</t>
+  </si>
+  <si>
+    <t>Aguardando validação do Matheus Seplag quanto ao conteúdo textual da consulta.</t>
+  </si>
+  <si>
+    <t>Aprovar conteúdo textual do Consulta</t>
+  </si>
+  <si>
+    <t>Alinhar com o Comitêo se conteúdo textual da consulta está conforme o desejado</t>
+  </si>
+  <si>
+    <t>06/04/2022</t>
+  </si>
+  <si>
+    <t>Aguardando validação do Matheus.</t>
+  </si>
+  <si>
+    <t>Atualização do conjunto de dados no repositório</t>
+  </si>
+  <si>
+    <t>Repassar para equipe do Comitê o fluxo de atualização dos dados</t>
+  </si>
+  <si>
+    <t>13/04/2022</t>
   </si>
 </sst>
 </file>
@@ -325,7 +361,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -349,9 +385,6 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -384,9 +417,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -400,6 +430,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -749,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,53 +805,53 @@
     <col min="3" max="3" width="33.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="23" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="21" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="23" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -815,26 +860,26 @@
       <c r="E2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="I2" s="8">
         <v>44588</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -843,10 +888,10 @@
       <c r="E3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>44596</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>44596</v>
       </c>
       <c r="H3" s="8">
@@ -855,16 +900,16 @@
       <c r="I3" s="8">
         <v>44596</v>
       </c>
-      <c r="J3" s="11"/>
-    </row>
-    <row r="4" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -873,10 +918,10 @@
       <c r="E4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <v>44596</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="17">
         <v>44600</v>
       </c>
       <c r="H4" s="8">
@@ -885,18 +930,18 @@
       <c r="I4" s="8">
         <v>44610</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:10" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>40</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -905,10 +950,10 @@
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <v>44593</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="17">
         <v>44603</v>
       </c>
       <c r="H5" s="8">
@@ -917,18 +962,18 @@
       <c r="I5" s="8">
         <v>44599</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -937,10 +982,10 @@
       <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="17">
         <v>44579</v>
       </c>
       <c r="H6" s="8">
@@ -949,18 +994,18 @@
       <c r="I6" s="8">
         <v>44588</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="J6" s="10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="7" t="s">
@@ -969,10 +1014,10 @@
       <c r="E7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <v>44601</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>44608</v>
       </c>
       <c r="H7" s="8">
@@ -981,18 +1026,18 @@
       <c r="I7" s="8">
         <v>44610</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -1001,10 +1046,10 @@
       <c r="E8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <v>44595</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="17">
         <v>44603</v>
       </c>
       <c r="H8" s="8">
@@ -1013,16 +1058,16 @@
       <c r="I8" s="8">
         <v>44610</v>
       </c>
-      <c r="J8" s="11"/>
-    </row>
-    <row r="9" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -1031,10 +1076,10 @@
       <c r="E9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <v>44609</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="17">
         <v>44613</v>
       </c>
       <c r="H9" s="8">
@@ -1043,44 +1088,46 @@
       <c r="I9" s="8">
         <v>44610</v>
       </c>
-      <c r="J9" s="11"/>
-    </row>
-    <row r="10" spans="1:10" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>44608</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>44613</v>
       </c>
       <c r="H10" s="8">
         <v>44608</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="11"/>
-    </row>
-    <row r="11" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="I10" s="8">
+        <v>44641</v>
+      </c>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>56</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -1089,152 +1136,168 @@
       <c r="E11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>44599</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="17">
         <v>44623</v>
       </c>
       <c r="H11" s="8">
         <v>44599</v>
       </c>
       <c r="I11" s="8">
-        <v>44623</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+        <v>44638</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>58</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>44623</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="17">
         <v>44627</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="H12" s="8">
+        <v>44624</v>
+      </c>
+      <c r="I12" s="8">
+        <v>44641</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>44614</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>44630</v>
       </c>
       <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="11"/>
-    </row>
-    <row r="14" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="I13" s="8">
+        <v>44630</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>44630</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="17">
         <v>44634</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="11"/>
-    </row>
-    <row r="15" spans="1:10" s="10" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="H14" s="8">
+        <v>44631</v>
+      </c>
+      <c r="I14" s="8">
+        <v>44637</v>
+      </c>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>44673</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="17">
         <v>44677</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="11"/>
-    </row>
-    <row r="16" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <v>44677</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="19">
         <v>44679</v>
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="11"/>
-    </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D17" s="7" t="s">
@@ -1243,151 +1306,195 @@
       <c r="E17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
       <c r="H17" s="8">
         <v>44606</v>
       </c>
       <c r="I17" s="8">
         <v>44607</v>
       </c>
-      <c r="J17" s="11" t="s">
+      <c r="J17" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="8">
         <v>44607</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="I18" s="8">
+        <v>44635</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <v>44613</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="11" t="s">
-        <v>60</v>
+      <c r="G19" s="17"/>
+      <c r="H19" s="8">
+        <v>44623</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="E20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>44627</v>
       </c>
-      <c r="G20" s="18">
+      <c r="G20" s="17">
         <v>44631</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="8">
+        <v>44623</v>
+      </c>
       <c r="I20" s="6"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="6"/>
+      <c r="J20" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" s="26">
+        <v>44657</v>
+      </c>
+      <c r="G21" s="26">
+        <v>44659</v>
+      </c>
+      <c r="H21" s="27" t="s">
+        <v>68</v>
+      </c>
       <c r="I21" s="6"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="12"/>
+      <c r="J21" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+      <c r="E22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>72</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="12"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="12"/>
+      <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="12"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="12"/>
+      <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1395,11 +1502,11 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="12"/>
+      <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
@@ -1407,11 +1514,11 @@
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="12"/>
+      <c r="J27" s="11"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D12 D19:D1048576 D15:D17">

</xml_diff>

<commit_message>
Atualiza plano de ação consulta vale
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Documents\tele-trabalho\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BC87D8-A55A-4F13-8947-0CE3B7B7BA5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="plano de ação" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -253,9 +252,6 @@
     <t>06/04/2022</t>
   </si>
   <si>
-    <t>Aguardando validação do Matheus.</t>
-  </si>
-  <si>
     <t>Atualização do conjunto de dados no repositório</t>
   </si>
   <si>
@@ -263,12 +259,31 @@
   </si>
   <si>
     <t>13/04/2022</t>
+  </si>
+  <si>
+    <t>19/05/2022</t>
+  </si>
+  <si>
+    <t>13/05/2022</t>
+  </si>
+  <si>
+    <t>Aguardando validação do Matheus.
+Dados validados pela equipe do Cômite</t>
+  </si>
+  <si>
+    <t>29/04/2022</t>
+  </si>
+  <si>
+    <t>09/05/2022</t>
+  </si>
+  <si>
+    <t>Consulta homologada com ressalvas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,7 +376,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -445,12 +460,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -791,11 +812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1273,9 @@
       <c r="C15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E15" s="7" t="s">
         <v>28</v>
       </c>
@@ -1263,7 +1286,9 @@
         <v>44677</v>
       </c>
       <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="31" t="s">
+        <v>76</v>
+      </c>
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1276,7 +1301,9 @@
       <c r="C16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="E16" s="7" t="s">
         <v>18</v>
       </c>
@@ -1287,8 +1314,12 @@
         <v>44679</v>
       </c>
       <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="10"/>
+      <c r="I16" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
@@ -1387,7 +1418,7 @@
         <v>53</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>18</v>
@@ -1401,12 +1432,14 @@
       <c r="H20" s="8">
         <v>44623</v>
       </c>
-      <c r="I20" s="6"/>
+      <c r="I20" s="30" t="s">
+        <v>72</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>48</v>
       </c>
@@ -1417,7 +1450,7 @@
         <v>67</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>55</v>
@@ -1431,9 +1464,11 @@
       <c r="H21" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="30" t="s">
+        <v>73</v>
+      </c>
       <c r="J21" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1441,23 +1476,29 @@
         <v>48</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="30" t="s">
+        <v>75</v>
+      </c>
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -1555,8 +1596,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" display="Link" xr:uid="{F3670588-9093-4D73-B964-2C29AC7BAFE5}"/>
-    <hyperlink ref="J5" r:id="rId2" display="v2" xr:uid="{1E85D808-692D-42AB-BE43-A82A9C0A4D7D}"/>
+    <hyperlink ref="J4" r:id="rId1" display="Link"/>
+    <hyperlink ref="J5" r:id="rId2" display="v2"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Atualiza plano de ação
</commit_message>
<xml_diff>
--- a/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
+++ b/espec018_recursos-acordo-judicial-vale/static/plano-acao-vale.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m13368964\Documents\tele-trabalho\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silviana\Documents\1. CGE\tele-trabalho\GIT\transparencia-mg\especificacoes-portal-transparencia\espec018_recursos-acordo-judicial-vale\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58199AE9-8FEB-4A60-B09D-C42F2C8384BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plano de ação" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
   <si>
     <t>Tarefa / Subtarefa</t>
   </si>
@@ -175,9 +176,6 @@
     <t>DTA/ Késia</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
     <t>v2
 Devido a mudanças na extração dos dados é necessário fazer uma nova revisão dos dados</t>
   </si>
@@ -278,12 +276,24 @@
   </si>
   <si>
     <t>Consulta homologada com ressalvas</t>
+  </si>
+  <si>
+    <t>Disponibilizar em Produção</t>
+  </si>
+  <si>
+    <t>Disponibilizar consulta em Produção</t>
+  </si>
+  <si>
+    <t>Disponibilizar em produção</t>
+  </si>
+  <si>
+    <t>Dados disponibilizados em produção com pendências conforme consta nos mantis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,6 +321,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -376,7 +387,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -466,12 +477,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="9">
     <dxf>
@@ -812,11 +826,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +998,7 @@
         <v>44599</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1048,7 +1062,7 @@
         <v>44610</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1149,7 +1163,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>13</v>
@@ -1170,7 +1184,7 @@
         <v>44638</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1181,7 +1195,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>13</v>
@@ -1202,7 +1216,7 @@
         <v>44641</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="9" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,7 +1227,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>13</v>
@@ -1241,7 +1255,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>13</v>
@@ -1287,7 +1301,7 @@
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J15" s="10"/>
     </row>
@@ -1302,7 +1316,7 @@
         <v>39</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>18</v>
@@ -1315,21 +1329,21 @@
       </c>
       <c r="H16" s="8"/>
       <c r="I16" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="9" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>13</v>
@@ -1346,24 +1360,24 @@
         <v>44607</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C18" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>54</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>55</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1374,18 +1388,18 @@
         <v>44635</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C19" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>13</v>
@@ -1401,21 +1415,21 @@
         <v>44623</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C20" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>13</v>
@@ -1433,27 +1447,27 @@
         <v>44623</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>67</v>
-      </c>
       <c r="D21" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21" s="26">
         <v>44657</v>
@@ -1462,24 +1476,24 @@
         <v>44659</v>
       </c>
       <c r="H21" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I21" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>70</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>13</v>
@@ -1488,30 +1502,44 @@
         <v>18</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="11"/>
+      <c r="I23" s="32">
+        <v>44734</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -1596,8 +1624,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" display="Link"/>
-    <hyperlink ref="J5" r:id="rId2" display="v2"/>
+    <hyperlink ref="J4" r:id="rId1" display="Link" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J5" r:id="rId2" display="v2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>